<commit_message>
update tabellen 5.1 in ontwikkeling
</commit_message>
<xml_diff>
--- a/ontwikkeling/concept 5.1.1/tabellen/objecten-classic/NLCS-OBJECTEN-BC-5.1.xlsx
+++ b/ontwikkeling/concept 5.1.1/tabellen/objecten-classic/NLCS-OBJECTEN-BC-5.1.xlsx
@@ -5,18 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stichtingcrow-my.sharepoint.com/personal/elisabeth_devries_crow_nl/Documents/Documents/GitHub/NLCS/ontwikkeling/concept 5.1.1/tabellen/objecten-classic/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\100289\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{2987A51F-03CC-438B-BE56-CDA25C396A8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F941098-8BA3-4689-8051-61B25A4C6D80}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{252DE946-895B-4F1B-B24D-94A6C544EF57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51720" yWindow="3270" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25905" yWindow="-3525" windowWidth="26010" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$BQ$38</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$BO$41</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="203">
   <si>
     <t>OMSCHRIJVING</t>
   </si>
@@ -182,6 +182,18 @@
     <t>VRKL_lang</t>
   </si>
   <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>KIND_VAN</t>
+  </si>
+  <si>
+    <t>URI</t>
+  </si>
+  <si>
+    <t>KIND_VAN_URI</t>
+  </si>
+  <si>
     <t>AANGRENZENDE CONSTRUCTIE_HOUT</t>
   </si>
   <si>
@@ -431,6 +443,9 @@
     <t>BC-STORTNAAD-SO</t>
   </si>
   <si>
+    <t>V-BC-STORTNAAD-SO</t>
+  </si>
+  <si>
     <t>http://digitalbuildingdata.tech/nlcs/def/776e2727-2419-4b54-90c4-695289c00064</t>
   </si>
   <si>
@@ -464,18 +479,6 @@
     <t>http://digitalbuildingdata.tech/nlcs/def/eb27111b-7e14-4597-a21c-abe2841941e2</t>
   </si>
   <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>KIND_VAN</t>
-  </si>
-  <si>
-    <t>URI</t>
-  </si>
-  <si>
-    <t>KIND_VAN_URI</t>
-  </si>
-  <si>
     <t>HOUT</t>
   </si>
   <si>
@@ -536,82 +539,82 @@
     <t>KABEL</t>
   </si>
   <si>
+    <t>*-**-BC-VOORSPANNING_MET AANHECHTING_KABEL</t>
+  </si>
+  <si>
+    <t>*-**-BC-VOORSPANNING_ZONDER AANHECHTING_KABEL</t>
+  </si>
+  <si>
+    <t>*-**-BC-BETONVORM_VSP_PREFAB</t>
+  </si>
+  <si>
+    <t>*-**-BC-VOORSPANNING_MET AANHECHTING_VERANKERING</t>
+  </si>
+  <si>
+    <t>*-**-BC-VOORSPANNING_ZONDER AANHECHTING_VERANKERING</t>
+  </si>
+  <si>
+    <t>*-**-BC-BETONVORM_BALLAST</t>
+  </si>
+  <si>
+    <t>*-**-BC-WAPENING_BIJLEGWAPENING</t>
+  </si>
+  <si>
+    <t>*-**-BC-BETONVORM_GEWAPEND</t>
+  </si>
+  <si>
+    <t>*-**-BC-WAPENING_HOOFDWAPENING</t>
+  </si>
+  <si>
     <t>*-**-BC-AANGRENZENDE CONSTRUCTIE_HOUT</t>
   </si>
   <si>
+    <t>*-**-BC-BETONVORM_IN HET WERK GESTORT</t>
+  </si>
+  <si>
+    <t>*-**-BC-BETONVORM_LICHT</t>
+  </si>
+  <si>
+    <t>*-**-BC-WAPENING_LOOPLIJN</t>
+  </si>
+  <si>
+    <t>*-**-BC-VOORSPANNING_MET AANHECHTING</t>
+  </si>
+  <si>
     <t>*-**-BC-AANGRENZENDE CONSTRUCTIE_METSELWERK</t>
   </si>
   <si>
+    <t>*-**-BC-BETONVORM_ONGEWAPEND</t>
+  </si>
+  <si>
+    <t>*-**-BC-BETONVORM_OWB</t>
+  </si>
+  <si>
+    <t>*-**-BC-BETONVORM_PREFAB</t>
+  </si>
+  <si>
     <t>*-**-BC-AANGRENZENDE CONSTRUCTIE_STAAL</t>
   </si>
   <si>
+    <t>*-**-BC-WAPENING_SUPPORT</t>
+  </si>
+  <si>
+    <t>*-**-BC-VOORSPANNING_SUPPORT</t>
+  </si>
+  <si>
+    <t>*-**-BC-BETONVORM_VSP</t>
+  </si>
+  <si>
+    <t>*-**-BC-BETONVORM_WERKVLOER</t>
+  </si>
+  <si>
     <t>*-**-BC-VOORSPANNING_ZONDER AANHECHTING</t>
   </si>
   <si>
-    <t>*-**-BC-VOORSPANNING_MET AANHECHTING</t>
-  </si>
-  <si>
     <t>*-**-BC-WAPENING</t>
   </si>
   <si>
     <t>*-**-BC-BETONVORM</t>
-  </si>
-  <si>
-    <t>*-**-BC-WAPENING_BIJLEGWAPENING</t>
-  </si>
-  <si>
-    <t>*-**-BC-WAPENING_LOOPLIJN</t>
-  </si>
-  <si>
-    <t>*-**-BC-WAPENING_HOOFDWAPENING</t>
-  </si>
-  <si>
-    <t>*-**-BC-WAPENING_SUPPORT</t>
-  </si>
-  <si>
-    <t>*-**-BC-BETONVORM_VSP</t>
-  </si>
-  <si>
-    <t>*-**-BC-BETONVORM_GEWAPEND</t>
-  </si>
-  <si>
-    <t>*-**-BC-BETONVORM_LICHT</t>
-  </si>
-  <si>
-    <t>*-**-BC-BETONVORM_PREFAB</t>
-  </si>
-  <si>
-    <t>*-**-BC-BETONVORM_BALLAST</t>
-  </si>
-  <si>
-    <t>*-**-BC-BETONVORM_OWB</t>
-  </si>
-  <si>
-    <t>*-**-BC-BETONVORM_ONGEWAPEND</t>
-  </si>
-  <si>
-    <t>*-**-BC-BETONVORM_WERKVLOER</t>
-  </si>
-  <si>
-    <t>*-**-BC-BETONVORM_IN HET WERK GESTORT</t>
-  </si>
-  <si>
-    <t>*-**-BC-VOORSPANNING_SUPPORT</t>
-  </si>
-  <si>
-    <t>*-**-BC-BETONVORM_VSP_PREFAB</t>
-  </si>
-  <si>
-    <t>*-**-BC-VOORSPANNING_ZONDER AANHECHTING_VERANKERING</t>
-  </si>
-  <si>
-    <t>*-**-BC-VOORSPANNING_ZONDER AANHECHTING_KABEL</t>
-  </si>
-  <si>
-    <t>*-**-BC-VOORSPANNING_MET AANHECHTING_KABEL</t>
-  </si>
-  <si>
-    <t>*-**-BC-VOORSPANNING_MET AANHECHTING_VERANKERING</t>
   </si>
   <si>
     <t>*-**-BC-AANGRENZENDE CONSTRUCTIE</t>
@@ -660,12 +663,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -680,8 +689,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -964,17 +974,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BG38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="X10" sqref="X10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="84.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="42.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="60.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="83.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="32.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:59" x14ac:dyDescent="0.25">
@@ -1050,7 +1069,7 @@
       <c r="X1" t="s">
         <v>15</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="Z1" t="s">
@@ -1144,48 +1163,48 @@
         <v>46</v>
       </c>
       <c r="BD1" t="s">
-        <v>141</v>
+        <v>47</v>
       </c>
       <c r="BE1" t="s">
-        <v>142</v>
+        <v>48</v>
       </c>
       <c r="BF1" t="s">
-        <v>143</v>
+        <v>49</v>
       </c>
       <c r="BG1" t="s">
-        <v>144</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G2" t="s">
         <v>2</v>
       </c>
       <c r="H2" t="s">
-        <v>119</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>191</v>
+        <v>123</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>192</v>
       </c>
       <c r="Z2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AA2">
         <v>7</v>
@@ -1203,10 +1222,10 @@
         <v>253</v>
       </c>
       <c r="AF2" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AG2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AH2">
         <v>7</v>
@@ -1224,10 +1243,10 @@
         <v>253</v>
       </c>
       <c r="AM2" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AN2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AO2">
         <v>7</v>
@@ -1245,10 +1264,10 @@
         <v>253</v>
       </c>
       <c r="AT2" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="AU2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AV2">
         <v>7</v>
@@ -1266,54 +1285,54 @@
         <v>253</v>
       </c>
       <c r="BA2" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="BD2">
         <v>2740</v>
       </c>
       <c r="BF2" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E3" t="s">
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G3" t="s">
         <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="I3" t="s">
         <v>6</v>
       </c>
       <c r="J3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="W3" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>165</v>
+        <v>55</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>175</v>
       </c>
       <c r="Z3" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AA3">
         <v>7</v>
@@ -1331,10 +1350,10 @@
         <v>253</v>
       </c>
       <c r="AF3" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AG3" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AH3">
         <v>7</v>
@@ -1352,10 +1371,10 @@
         <v>253</v>
       </c>
       <c r="AM3" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AN3" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AO3">
         <v>7</v>
@@ -1373,10 +1392,10 @@
         <v>253</v>
       </c>
       <c r="AT3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="AU3" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AV3">
         <v>7</v>
@@ -1394,7 +1413,7 @@
         <v>253</v>
       </c>
       <c r="BA3" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="BD3">
         <v>2742</v>
@@ -1403,51 +1422,51 @@
         <v>2740</v>
       </c>
       <c r="BF3" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="BG3" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E4" t="s">
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G4" t="s">
         <v>2</v>
       </c>
       <c r="H4" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="I4" t="s">
         <v>6</v>
       </c>
       <c r="J4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="W4" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>166</v>
+        <v>62</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>180</v>
       </c>
       <c r="Z4" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AA4">
         <v>7</v>
@@ -1465,10 +1484,10 @@
         <v>253</v>
       </c>
       <c r="AF4" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AG4" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AH4">
         <v>7</v>
@@ -1486,10 +1505,10 @@
         <v>253</v>
       </c>
       <c r="AM4" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AN4" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AO4">
         <v>7</v>
@@ -1507,10 +1526,10 @@
         <v>253</v>
       </c>
       <c r="AT4" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="AU4" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AV4">
         <v>7</v>
@@ -1528,7 +1547,7 @@
         <v>253</v>
       </c>
       <c r="BA4" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="BD4">
         <v>2743</v>
@@ -1537,51 +1556,51 @@
         <v>2740</v>
       </c>
       <c r="BF4" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="BG4" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E5" t="s">
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G5" t="s">
         <v>2</v>
       </c>
       <c r="H5" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="I5" t="s">
         <v>6</v>
       </c>
       <c r="J5" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="W5" t="s">
-        <v>61</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>167</v>
+        <v>65</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>184</v>
       </c>
       <c r="Z5" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AA5">
         <v>7</v>
@@ -1599,10 +1618,10 @@
         <v>253</v>
       </c>
       <c r="AF5" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AG5" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AH5">
         <v>7</v>
@@ -1620,10 +1639,10 @@
         <v>253</v>
       </c>
       <c r="AM5" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AN5" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AO5">
         <v>7</v>
@@ -1641,10 +1660,10 @@
         <v>253</v>
       </c>
       <c r="AT5" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="AU5" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AV5">
         <v>7</v>
@@ -1662,7 +1681,7 @@
         <v>253</v>
       </c>
       <c r="BA5" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="BD5">
         <v>2741</v>
@@ -1671,45 +1690,45 @@
         <v>2740</v>
       </c>
       <c r="BF5" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="BG5" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E6" t="s">
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G6" t="s">
         <v>2</v>
       </c>
       <c r="H6" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="W6" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>171</v>
+        <v>80</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>191</v>
       </c>
       <c r="Z6" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AA6">
         <v>40</v>
@@ -1727,10 +1746,10 @@
         <v>254</v>
       </c>
       <c r="AF6" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AG6" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="AH6">
         <v>40</v>
@@ -1748,10 +1767,10 @@
         <v>254</v>
       </c>
       <c r="AM6" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AN6" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="AO6">
         <v>40</v>
@@ -1769,10 +1788,10 @@
         <v>254</v>
       </c>
       <c r="AT6" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="AU6" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="AV6">
         <v>40</v>
@@ -1790,51 +1809,51 @@
         <v>254</v>
       </c>
       <c r="BA6" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="BD6">
         <v>2712</v>
       </c>
       <c r="BF6" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E7" t="s">
         <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G7" t="s">
         <v>2</v>
       </c>
       <c r="H7" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="I7" t="s">
         <v>6</v>
       </c>
       <c r="J7" t="s">
-        <v>158</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>180</v>
+        <v>159</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>171</v>
       </c>
       <c r="Z7" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AA7">
         <v>40</v>
@@ -1852,10 +1871,10 @@
         <v>254</v>
       </c>
       <c r="AF7" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AG7" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="AH7">
         <v>40</v>
@@ -1873,10 +1892,10 @@
         <v>254</v>
       </c>
       <c r="AM7" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AN7" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="AO7">
         <v>40</v>
@@ -1894,10 +1913,10 @@
         <v>254</v>
       </c>
       <c r="AT7" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="AU7" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="AV7">
         <v>40</v>
@@ -1915,7 +1934,7 @@
         <v>254</v>
       </c>
       <c r="BA7" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="BD7">
         <v>2720</v>
@@ -1924,48 +1943,48 @@
         <v>2712</v>
       </c>
       <c r="BF7" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="BG7" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E8" t="s">
         <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G8" t="s">
         <v>2</v>
       </c>
       <c r="H8" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="I8" t="s">
         <v>6</v>
       </c>
       <c r="J8" t="s">
-        <v>155</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>177</v>
+        <v>156</v>
+      </c>
+      <c r="Y8" s="1" t="s">
+        <v>173</v>
       </c>
       <c r="Z8" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AA8">
         <v>40</v>
@@ -1983,10 +2002,10 @@
         <v>254</v>
       </c>
       <c r="AF8" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AG8" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="AH8">
         <v>40</v>
@@ -2004,10 +2023,10 @@
         <v>254</v>
       </c>
       <c r="AM8" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AN8" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="AO8">
         <v>40</v>
@@ -2025,10 +2044,10 @@
         <v>254</v>
       </c>
       <c r="AT8" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="AU8" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="AV8">
         <v>40</v>
@@ -2046,7 +2065,7 @@
         <v>254</v>
       </c>
       <c r="BA8" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="BD8">
         <v>2718</v>
@@ -2055,48 +2074,48 @@
         <v>2712</v>
       </c>
       <c r="BF8" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="BG8" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C9" t="s">
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E9" t="s">
         <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G9" t="s">
         <v>2</v>
       </c>
       <c r="H9" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="I9" t="s">
         <v>6</v>
       </c>
       <c r="J9" t="s">
-        <v>162</v>
-      </c>
-      <c r="Y9" t="s">
-        <v>184</v>
+        <v>163</v>
+      </c>
+      <c r="Y9" s="1" t="s">
+        <v>176</v>
       </c>
       <c r="Z9" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AA9">
         <v>40</v>
@@ -2114,10 +2133,10 @@
         <v>254</v>
       </c>
       <c r="AF9" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AG9" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="AH9">
         <v>40</v>
@@ -2135,10 +2154,10 @@
         <v>254</v>
       </c>
       <c r="AM9" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AN9" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="AO9">
         <v>40</v>
@@ -2156,10 +2175,10 @@
         <v>254</v>
       </c>
       <c r="AT9" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="AU9" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="AV9">
         <v>40</v>
@@ -2177,7 +2196,7 @@
         <v>254</v>
       </c>
       <c r="BA9" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="BD9">
         <v>2880</v>
@@ -2186,48 +2205,48 @@
         <v>2712</v>
       </c>
       <c r="BF9" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="BG9" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C10" t="s">
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E10" t="s">
         <v>2</v>
       </c>
       <c r="F10" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G10" t="s">
         <v>2</v>
       </c>
       <c r="H10" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="I10" t="s">
         <v>6</v>
       </c>
       <c r="J10" t="s">
-        <v>156</v>
-      </c>
-      <c r="Y10" t="s">
-        <v>178</v>
+        <v>157</v>
+      </c>
+      <c r="Y10" s="1" t="s">
+        <v>177</v>
       </c>
       <c r="Z10" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AA10">
         <v>40</v>
@@ -2245,10 +2264,10 @@
         <v>254</v>
       </c>
       <c r="AF10" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AG10" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="AH10">
         <v>40</v>
@@ -2266,10 +2285,10 @@
         <v>254</v>
       </c>
       <c r="AM10" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AN10" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="AO10">
         <v>40</v>
@@ -2287,10 +2306,10 @@
         <v>254</v>
       </c>
       <c r="AT10" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="AU10" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="AV10">
         <v>40</v>
@@ -2308,7 +2327,7 @@
         <v>254</v>
       </c>
       <c r="BA10" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="BD10">
         <v>2713</v>
@@ -2317,48 +2336,48 @@
         <v>2712</v>
       </c>
       <c r="BF10" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="BG10" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E11" t="s">
         <v>2</v>
       </c>
       <c r="F11" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G11" t="s">
         <v>2</v>
       </c>
       <c r="H11" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="I11" t="s">
         <v>6</v>
       </c>
       <c r="J11" t="s">
-        <v>160</v>
-      </c>
-      <c r="Y11" t="s">
-        <v>182</v>
+        <v>161</v>
+      </c>
+      <c r="Y11" s="1" t="s">
+        <v>181</v>
       </c>
       <c r="Z11" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AA11">
         <v>40</v>
@@ -2376,10 +2395,10 @@
         <v>254</v>
       </c>
       <c r="AF11" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AG11" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="AH11">
         <v>40</v>
@@ -2397,10 +2416,10 @@
         <v>254</v>
       </c>
       <c r="AM11" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AN11" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="AO11">
         <v>40</v>
@@ -2418,10 +2437,10 @@
         <v>254</v>
       </c>
       <c r="AT11" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="AU11" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="AV11">
         <v>40</v>
@@ -2439,7 +2458,7 @@
         <v>254</v>
       </c>
       <c r="BA11" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="BD11">
         <v>2719</v>
@@ -2448,48 +2467,48 @@
         <v>2712</v>
       </c>
       <c r="BF11" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="BG11" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B12" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E12" t="s">
         <v>2</v>
       </c>
       <c r="F12" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G12" t="s">
         <v>2</v>
       </c>
       <c r="H12" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="I12" t="s">
         <v>6</v>
       </c>
       <c r="J12" t="s">
-        <v>159</v>
-      </c>
-      <c r="Y12" t="s">
-        <v>181</v>
+        <v>160</v>
+      </c>
+      <c r="Y12" s="1" t="s">
+        <v>182</v>
       </c>
       <c r="Z12" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AA12">
         <v>40</v>
@@ -2507,10 +2526,10 @@
         <v>254</v>
       </c>
       <c r="AF12" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AG12" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="AH12">
         <v>40</v>
@@ -2528,10 +2547,10 @@
         <v>254</v>
       </c>
       <c r="AM12" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AN12" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="AO12">
         <v>40</v>
@@ -2549,10 +2568,10 @@
         <v>254</v>
       </c>
       <c r="AT12" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="AU12" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="AV12">
         <v>40</v>
@@ -2570,7 +2589,7 @@
         <v>254</v>
       </c>
       <c r="BA12" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="BD12">
         <v>2717</v>
@@ -2579,48 +2598,48 @@
         <v>2712</v>
       </c>
       <c r="BF12" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="BG12" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B13" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C13" t="s">
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E13" t="s">
         <v>2</v>
       </c>
       <c r="F13" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G13" t="s">
         <v>2</v>
       </c>
       <c r="H13" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="I13" t="s">
         <v>6</v>
       </c>
       <c r="J13" t="s">
-        <v>157</v>
-      </c>
-      <c r="Y13" t="s">
-        <v>179</v>
+        <v>158</v>
+      </c>
+      <c r="Y13" s="1" t="s">
+        <v>183</v>
       </c>
       <c r="Z13" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AA13">
         <v>40</v>
@@ -2638,10 +2657,10 @@
         <v>254</v>
       </c>
       <c r="AF13" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AG13" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="AH13">
         <v>40</v>
@@ -2659,10 +2678,10 @@
         <v>254</v>
       </c>
       <c r="AM13" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AN13" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="AO13">
         <v>40</v>
@@ -2680,10 +2699,10 @@
         <v>254</v>
       </c>
       <c r="AT13" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="AU13" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="AV13">
         <v>40</v>
@@ -2701,7 +2720,7 @@
         <v>253</v>
       </c>
       <c r="BA13" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="BD13">
         <v>2714</v>
@@ -2710,48 +2729,48 @@
         <v>2712</v>
       </c>
       <c r="BF13" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="BG13" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C14" t="s">
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E14" t="s">
         <v>2</v>
       </c>
       <c r="F14" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G14" t="s">
         <v>2</v>
       </c>
       <c r="H14" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="I14" t="s">
         <v>6</v>
       </c>
       <c r="J14" t="s">
-        <v>154</v>
-      </c>
-      <c r="Y14" t="s">
-        <v>176</v>
+        <v>155</v>
+      </c>
+      <c r="Y14" s="1" t="s">
+        <v>187</v>
       </c>
       <c r="Z14" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AA14">
         <v>40</v>
@@ -2769,10 +2788,10 @@
         <v>254</v>
       </c>
       <c r="AF14" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AG14" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="AH14">
         <v>40</v>
@@ -2790,10 +2809,10 @@
         <v>254</v>
       </c>
       <c r="AM14" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AN14" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="AO14">
         <v>40</v>
@@ -2811,10 +2830,10 @@
         <v>254</v>
       </c>
       <c r="AT14" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="AU14" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="AV14">
         <v>40</v>
@@ -2832,7 +2851,7 @@
         <v>254</v>
       </c>
       <c r="BA14" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="BD14">
         <v>2715</v>
@@ -2841,54 +2860,54 @@
         <v>2712</v>
       </c>
       <c r="BF14" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="BG14" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B15" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C15" t="s">
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E15" t="s">
         <v>2</v>
       </c>
       <c r="F15" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G15" t="s">
         <v>2</v>
       </c>
       <c r="H15" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="I15" t="s">
         <v>6</v>
       </c>
       <c r="J15" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="K15" t="s">
         <v>6</v>
       </c>
       <c r="L15" t="s">
-        <v>157</v>
-      </c>
-      <c r="Y15" t="s">
-        <v>186</v>
+        <v>158</v>
+      </c>
+      <c r="Y15" s="1" t="s">
+        <v>168</v>
       </c>
       <c r="Z15" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AA15">
         <v>40</v>
@@ -2906,10 +2925,10 @@
         <v>253</v>
       </c>
       <c r="AF15" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AG15" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="AH15">
         <v>40</v>
@@ -2927,10 +2946,10 @@
         <v>253</v>
       </c>
       <c r="AM15" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AN15" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="AO15">
         <v>40</v>
@@ -2948,10 +2967,10 @@
         <v>253</v>
       </c>
       <c r="AT15" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="AU15" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="AV15">
         <v>40</v>
@@ -2969,7 +2988,7 @@
         <v>253</v>
       </c>
       <c r="BA15" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="BD15">
         <v>2716</v>
@@ -2978,48 +2997,48 @@
         <v>2715</v>
       </c>
       <c r="BF15" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="BG15" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
       </c>
       <c r="D16" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E16" t="s">
         <v>2</v>
       </c>
       <c r="F16" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G16" t="s">
         <v>2</v>
       </c>
       <c r="H16" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="I16" t="s">
         <v>6</v>
       </c>
       <c r="J16" t="s">
-        <v>161</v>
-      </c>
-      <c r="Y16" t="s">
-        <v>183</v>
+        <v>162</v>
+      </c>
+      <c r="Y16" s="1" t="s">
+        <v>188</v>
       </c>
       <c r="Z16" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AA16">
         <v>10</v>
@@ -3037,10 +3056,10 @@
         <v>254</v>
       </c>
       <c r="AF16" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AG16" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AH16">
         <v>10</v>
@@ -3058,10 +3077,10 @@
         <v>254</v>
       </c>
       <c r="AM16" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AN16" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AO16">
         <v>10</v>
@@ -3079,10 +3098,10 @@
         <v>254</v>
       </c>
       <c r="AT16" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="AU16" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AV16">
         <v>10</v>
@@ -3100,7 +3119,7 @@
         <v>254</v>
       </c>
       <c r="BA16" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="BD16">
         <v>2721</v>
@@ -3109,42 +3128,42 @@
         <v>2712</v>
       </c>
       <c r="BF16" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="BG16" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E17" t="s">
         <v>2</v>
       </c>
       <c r="F17" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G17" t="s">
         <v>2</v>
       </c>
       <c r="H17" t="s">
-        <v>135</v>
-      </c>
-      <c r="Y17" t="s">
-        <v>199</v>
+        <v>140</v>
+      </c>
+      <c r="Y17" s="1" t="s">
+        <v>200</v>
       </c>
       <c r="Z17" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AA17">
         <v>7</v>
@@ -3162,10 +3181,10 @@
         <v>253</v>
       </c>
       <c r="AF17" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AG17" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AH17">
         <v>7</v>
@@ -3183,10 +3202,10 @@
         <v>253</v>
       </c>
       <c r="AM17" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AN17" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AO17">
         <v>7</v>
@@ -3204,10 +3223,10 @@
         <v>253</v>
       </c>
       <c r="AT17" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="AU17" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AV17">
         <v>7</v>
@@ -3225,45 +3244,45 @@
         <v>253</v>
       </c>
       <c r="BA17" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="BD17">
         <v>3009</v>
       </c>
       <c r="BF17" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
     </row>
     <row r="18" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="B18" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C18" t="s">
         <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E18" t="s">
         <v>2</v>
       </c>
       <c r="F18" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G18" t="s">
         <v>2</v>
       </c>
       <c r="H18" t="s">
-        <v>133</v>
-      </c>
-      <c r="Y18" t="s">
-        <v>198</v>
+        <v>138</v>
+      </c>
+      <c r="Y18" s="1" t="s">
+        <v>199</v>
       </c>
       <c r="Z18" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AA18">
         <v>30</v>
@@ -3281,10 +3300,10 @@
         <v>254</v>
       </c>
       <c r="AF18" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AG18" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AH18">
         <v>30</v>
@@ -3302,10 +3321,10 @@
         <v>254</v>
       </c>
       <c r="AM18" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AN18" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AO18">
         <v>30</v>
@@ -3323,10 +3342,10 @@
         <v>254</v>
       </c>
       <c r="AT18" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="AU18" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AV18">
         <v>30</v>
@@ -3344,45 +3363,45 @@
         <v>254</v>
       </c>
       <c r="BA18" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="BD18">
         <v>2725</v>
       </c>
       <c r="BF18" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
     </row>
     <row r="19" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="B19" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C19" t="s">
         <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E19" t="s">
         <v>2</v>
       </c>
       <c r="F19" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G19" t="s">
         <v>2</v>
       </c>
       <c r="H19" t="s">
-        <v>123</v>
-      </c>
-      <c r="Y19" t="s">
-        <v>194</v>
+        <v>127</v>
+      </c>
+      <c r="Y19" s="1" t="s">
+        <v>195</v>
       </c>
       <c r="Z19" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AA19">
         <v>170</v>
@@ -3400,10 +3419,10 @@
         <v>253</v>
       </c>
       <c r="AF19" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AG19" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="AH19">
         <v>170</v>
@@ -3421,10 +3440,10 @@
         <v>253</v>
       </c>
       <c r="AM19" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AN19" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="AO19">
         <v>170</v>
@@ -3442,10 +3461,10 @@
         <v>253</v>
       </c>
       <c r="AT19" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="AU19" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="AV19">
         <v>170</v>
@@ -3463,45 +3482,45 @@
         <v>253</v>
       </c>
       <c r="BA19" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="BD19">
         <v>2746</v>
       </c>
       <c r="BF19" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
     </row>
     <row r="20" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B20" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E20" t="s">
         <v>2</v>
       </c>
       <c r="F20" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G20" t="s">
         <v>2</v>
       </c>
       <c r="H20" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y20" t="s">
-        <v>192</v>
+        <v>124</v>
+      </c>
+      <c r="Y20" s="1" t="s">
+        <v>193</v>
       </c>
       <c r="Z20" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AA20">
         <v>30</v>
@@ -3519,10 +3538,10 @@
         <v>254</v>
       </c>
       <c r="AF20" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AG20" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AH20">
         <v>30</v>
@@ -3540,10 +3559,10 @@
         <v>254</v>
       </c>
       <c r="AM20" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AN20" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AO20">
         <v>30</v>
@@ -3561,10 +3580,10 @@
         <v>254</v>
       </c>
       <c r="AT20" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="AU20" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AV20">
         <v>30</v>
@@ -3582,45 +3601,45 @@
         <v>254</v>
       </c>
       <c r="BA20" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="BD20">
         <v>2726</v>
       </c>
       <c r="BF20" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
     </row>
     <row r="21" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="B21" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E21" t="s">
         <v>2</v>
       </c>
       <c r="F21" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G21" t="s">
         <v>2</v>
       </c>
       <c r="H21" t="s">
-        <v>137</v>
-      </c>
-      <c r="Y21" t="s">
-        <v>200</v>
+        <v>142</v>
+      </c>
+      <c r="Y21" s="1" t="s">
+        <v>201</v>
       </c>
       <c r="Z21" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AA21">
         <v>7</v>
@@ -3638,10 +3657,10 @@
         <v>255</v>
       </c>
       <c r="AF21" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AG21" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AH21">
         <v>7</v>
@@ -3659,10 +3678,10 @@
         <v>255</v>
       </c>
       <c r="AM21" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AN21" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AO21">
         <v>7</v>
@@ -3680,10 +3699,10 @@
         <v>255</v>
       </c>
       <c r="AT21" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="AU21" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AV21">
         <v>7</v>
@@ -3701,45 +3720,45 @@
         <v>255</v>
       </c>
       <c r="BA21" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="BD21">
         <v>2744</v>
       </c>
       <c r="BF21" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
     </row>
     <row r="22" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="B22" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C22" t="s">
         <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E22" t="s">
         <v>2</v>
       </c>
       <c r="F22" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G22" t="s">
         <v>2</v>
       </c>
       <c r="H22" t="s">
-        <v>131</v>
-      </c>
-      <c r="Y22" t="s">
-        <v>197</v>
+        <v>136</v>
+      </c>
+      <c r="Y22" s="1" t="s">
+        <v>198</v>
       </c>
       <c r="Z22" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AA22">
         <v>170</v>
@@ -3757,10 +3776,10 @@
         <v>253</v>
       </c>
       <c r="AF22" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AG22" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="AH22">
         <v>170</v>
@@ -3778,10 +3797,10 @@
         <v>253</v>
       </c>
       <c r="AM22" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AN22" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="AO22">
         <v>170</v>
@@ -3799,10 +3818,10 @@
         <v>253</v>
       </c>
       <c r="AT22" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="AU22" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="AV22">
         <v>170</v>
@@ -3820,45 +3839,45 @@
         <v>253</v>
       </c>
       <c r="BA22" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="BD22">
         <v>2745</v>
       </c>
       <c r="BF22" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
     </row>
     <row r="23" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B23" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C23" t="s">
         <v>2</v>
       </c>
       <c r="D23" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E23" t="s">
         <v>2</v>
       </c>
       <c r="F23" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G23" t="s">
         <v>2</v>
       </c>
       <c r="H23" t="s">
-        <v>125</v>
-      </c>
-      <c r="Y23" t="s">
-        <v>195</v>
+        <v>129</v>
+      </c>
+      <c r="Y23" s="1" t="s">
+        <v>196</v>
       </c>
       <c r="Z23" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AA23">
         <v>10</v>
@@ -3876,10 +3895,10 @@
         <v>254</v>
       </c>
       <c r="AF23" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="AG23" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AH23">
         <v>10</v>
@@ -3897,10 +3916,10 @@
         <v>254</v>
       </c>
       <c r="AM23" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="AN23" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AO23">
         <v>10</v>
@@ -3918,10 +3937,10 @@
         <v>254</v>
       </c>
       <c r="AT23" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="AU23" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AV23">
         <v>10</v>
@@ -3939,45 +3958,45 @@
         <v>254</v>
       </c>
       <c r="BA23" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="BD23">
         <v>2723</v>
       </c>
       <c r="BF23" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
     </row>
     <row r="24" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="B24" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C24" t="s">
         <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E24" t="s">
         <v>2</v>
       </c>
       <c r="F24" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G24" t="s">
         <v>2</v>
       </c>
       <c r="H24" t="s">
-        <v>128</v>
-      </c>
-      <c r="Y24" t="s">
-        <v>196</v>
+        <v>132</v>
+      </c>
+      <c r="Y24" s="1" t="s">
+        <v>197</v>
       </c>
       <c r="Z24" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AA24">
         <v>10</v>
@@ -3995,10 +4014,10 @@
         <v>254</v>
       </c>
       <c r="AF24" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="AG24" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AH24">
         <v>10</v>
@@ -4016,10 +4035,10 @@
         <v>254</v>
       </c>
       <c r="AM24" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="AN24" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AO24">
         <v>10</v>
@@ -4037,10 +4056,10 @@
         <v>254</v>
       </c>
       <c r="AT24" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="AU24" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AV24">
         <v>10</v>
@@ -4058,45 +4077,45 @@
         <v>254</v>
       </c>
       <c r="BA24" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="BD24">
         <v>2722</v>
       </c>
       <c r="BF24" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
     </row>
     <row r="25" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="B25" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C25" t="s">
         <v>2</v>
       </c>
       <c r="D25" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E25" t="s">
         <v>2</v>
       </c>
       <c r="F25" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G25" t="s">
         <v>2</v>
       </c>
       <c r="H25" t="s">
-        <v>139</v>
-      </c>
-      <c r="Y25" t="s">
-        <v>201</v>
+        <v>144</v>
+      </c>
+      <c r="Y25" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="Z25" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AA25">
         <v>30</v>
@@ -4114,10 +4133,10 @@
         <v>254</v>
       </c>
       <c r="AF25" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AG25" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AH25">
         <v>30</v>
@@ -4135,10 +4154,10 @@
         <v>254</v>
       </c>
       <c r="AM25" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AN25" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AO25">
         <v>30</v>
@@ -4156,10 +4175,10 @@
         <v>254</v>
       </c>
       <c r="AT25" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="AU25" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AV25">
         <v>30</v>
@@ -4177,45 +4196,45 @@
         <v>254</v>
       </c>
       <c r="BA25" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="BD25">
         <v>2724</v>
       </c>
       <c r="BF25" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
     </row>
     <row r="26" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="B26" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C26" t="s">
         <v>2</v>
       </c>
       <c r="D26" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E26" t="s">
         <v>2</v>
       </c>
       <c r="F26" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G26" t="s">
         <v>2</v>
       </c>
       <c r="H26" t="s">
-        <v>122</v>
-      </c>
-      <c r="Y26" t="s">
-        <v>193</v>
+        <v>126</v>
+      </c>
+      <c r="Y26" s="1" t="s">
+        <v>194</v>
       </c>
       <c r="Z26" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AA26">
         <v>180</v>
@@ -4233,10 +4252,10 @@
         <v>254</v>
       </c>
       <c r="AF26" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AG26" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="AH26">
         <v>180</v>
@@ -4254,10 +4273,10 @@
         <v>254</v>
       </c>
       <c r="AM26" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AN26" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="AO26">
         <v>180</v>
@@ -4275,10 +4294,10 @@
         <v>254</v>
       </c>
       <c r="AT26" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="AU26" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="AV26">
         <v>180</v>
@@ -4296,54 +4315,54 @@
         <v>254</v>
       </c>
       <c r="BA26" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="BD26">
         <v>2732</v>
       </c>
       <c r="BF26" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B27" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C27" t="s">
         <v>2</v>
       </c>
       <c r="D27" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E27" t="s">
         <v>2</v>
       </c>
       <c r="F27" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G27" t="s">
         <v>2</v>
       </c>
       <c r="H27" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="I27" t="s">
         <v>6</v>
       </c>
       <c r="J27" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="X27" t="s">
-        <v>69</v>
-      </c>
-      <c r="Y27" t="s">
-        <v>169</v>
+        <v>73</v>
+      </c>
+      <c r="Y27" s="1" t="s">
+        <v>179</v>
       </c>
       <c r="Z27" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AA27">
         <v>180</v>
@@ -4361,10 +4380,10 @@
         <v>254</v>
       </c>
       <c r="AF27" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AG27" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="AH27">
         <v>180</v>
@@ -4382,10 +4401,10 @@
         <v>254</v>
       </c>
       <c r="AM27" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AN27" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="AO27">
         <v>180</v>
@@ -4403,10 +4422,10 @@
         <v>254</v>
       </c>
       <c r="AT27" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="AU27" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="AV27">
         <v>180</v>
@@ -4424,7 +4443,7 @@
         <v>254</v>
       </c>
       <c r="BA27" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="BD27">
         <v>2736</v>
@@ -4433,54 +4452,54 @@
         <v>2732</v>
       </c>
       <c r="BF27" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="BG27" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B28" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C28" t="s">
         <v>2</v>
       </c>
       <c r="D28" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E28" t="s">
         <v>2</v>
       </c>
       <c r="F28" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G28" t="s">
         <v>2</v>
       </c>
       <c r="H28" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="I28" t="s">
         <v>6</v>
       </c>
       <c r="J28" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="K28" t="s">
         <v>6</v>
       </c>
       <c r="L28" t="s">
-        <v>164</v>
-      </c>
-      <c r="Y28" t="s">
-        <v>189</v>
+        <v>165</v>
+      </c>
+      <c r="Y28" s="1" t="s">
+        <v>166</v>
       </c>
       <c r="Z28" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AA28">
         <v>180</v>
@@ -4498,10 +4517,10 @@
         <v>254</v>
       </c>
       <c r="AF28" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="AG28" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="AH28">
         <v>180</v>
@@ -4519,10 +4538,10 @@
         <v>254</v>
       </c>
       <c r="AM28" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="AN28" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="AO28">
         <v>180</v>
@@ -4540,10 +4559,10 @@
         <v>254</v>
       </c>
       <c r="AT28" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="AU28" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="AV28">
         <v>180</v>
@@ -4561,7 +4580,7 @@
         <v>254</v>
       </c>
       <c r="BA28" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="BD28">
         <v>2737</v>
@@ -4570,54 +4589,54 @@
         <v>2736</v>
       </c>
       <c r="BF28" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="BG28" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="B29" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C29" t="s">
         <v>2</v>
       </c>
       <c r="D29" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E29" t="s">
         <v>2</v>
       </c>
       <c r="F29" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G29" t="s">
         <v>2</v>
       </c>
       <c r="H29" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="I29" t="s">
         <v>6</v>
       </c>
       <c r="J29" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="K29" t="s">
         <v>6</v>
       </c>
       <c r="L29" t="s">
-        <v>163</v>
-      </c>
-      <c r="Y29" t="s">
-        <v>190</v>
+        <v>164</v>
+      </c>
+      <c r="Y29" s="1" t="s">
+        <v>169</v>
       </c>
       <c r="Z29" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AA29">
         <v>180</v>
@@ -4635,10 +4654,10 @@
         <v>254</v>
       </c>
       <c r="AF29" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AG29" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="AH29">
         <v>180</v>
@@ -4656,10 +4675,10 @@
         <v>254</v>
       </c>
       <c r="AM29" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AN29" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AO29">
         <v>180</v>
@@ -4677,10 +4696,10 @@
         <v>254</v>
       </c>
       <c r="AT29" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="AU29" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AV29">
         <v>180</v>
@@ -4698,7 +4717,7 @@
         <v>254</v>
       </c>
       <c r="BA29" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="BD29">
         <v>2738</v>
@@ -4707,48 +4726,48 @@
         <v>2736</v>
       </c>
       <c r="BF29" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="BG29" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B30" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C30" t="s">
         <v>2</v>
       </c>
       <c r="D30" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E30" t="s">
         <v>2</v>
       </c>
       <c r="F30" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G30" t="s">
         <v>2</v>
       </c>
       <c r="H30" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="I30" t="s">
         <v>6</v>
       </c>
       <c r="J30" t="s">
-        <v>153</v>
-      </c>
-      <c r="Y30" t="s">
-        <v>185</v>
+        <v>154</v>
+      </c>
+      <c r="Y30" s="1" t="s">
+        <v>186</v>
       </c>
       <c r="Z30" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AA30">
         <v>7</v>
@@ -4766,10 +4785,10 @@
         <v>254</v>
       </c>
       <c r="AF30" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AG30" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="AH30">
         <v>7</v>
@@ -4787,10 +4806,10 @@
         <v>254</v>
       </c>
       <c r="AM30" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AN30" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AO30">
         <v>7</v>
@@ -4808,10 +4827,10 @@
         <v>254</v>
       </c>
       <c r="AT30" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="AU30" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AV30">
         <v>7</v>
@@ -4829,7 +4848,7 @@
         <v>254</v>
       </c>
       <c r="BA30" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="BD30">
         <v>2739</v>
@@ -4838,51 +4857,51 @@
         <v>2732</v>
       </c>
       <c r="BF30" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="BG30" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B31" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C31" t="s">
         <v>2</v>
       </c>
       <c r="D31" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E31" t="s">
         <v>2</v>
       </c>
       <c r="F31" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G31" t="s">
         <v>2</v>
       </c>
       <c r="H31" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="I31" t="s">
         <v>6</v>
       </c>
       <c r="J31" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="X31" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y31" t="s">
-        <v>168</v>
+        <v>68</v>
+      </c>
+      <c r="Y31" s="1" t="s">
+        <v>189</v>
       </c>
       <c r="Z31" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AA31">
         <v>180</v>
@@ -4900,10 +4919,10 @@
         <v>254</v>
       </c>
       <c r="AF31" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AG31" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="AH31">
         <v>180</v>
@@ -4921,10 +4940,10 @@
         <v>254</v>
       </c>
       <c r="AM31" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AN31" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="AO31">
         <v>180</v>
@@ -4942,10 +4961,10 @@
         <v>254</v>
       </c>
       <c r="AT31" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="AU31" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="AV31">
         <v>180</v>
@@ -4963,7 +4982,7 @@
         <v>254</v>
       </c>
       <c r="BA31" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="BD31">
         <v>2733</v>
@@ -4972,54 +4991,54 @@
         <v>2732</v>
       </c>
       <c r="BF31" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="BG31" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="B32" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C32" t="s">
         <v>2</v>
       </c>
       <c r="D32" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E32" t="s">
         <v>2</v>
       </c>
       <c r="F32" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G32" t="s">
         <v>2</v>
       </c>
       <c r="H32" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="I32" t="s">
         <v>6</v>
       </c>
       <c r="J32" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="K32" t="s">
         <v>6</v>
       </c>
       <c r="L32" t="s">
-        <v>164</v>
-      </c>
-      <c r="Y32" t="s">
-        <v>188</v>
+        <v>165</v>
+      </c>
+      <c r="Y32" s="1" t="s">
+        <v>167</v>
       </c>
       <c r="Z32" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AA32">
         <v>180</v>
@@ -5037,10 +5056,10 @@
         <v>254</v>
       </c>
       <c r="AF32" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AG32" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="AH32">
         <v>180</v>
@@ -5058,10 +5077,10 @@
         <v>254</v>
       </c>
       <c r="AM32" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AN32" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="AO32">
         <v>180</v>
@@ -5079,10 +5098,10 @@
         <v>254</v>
       </c>
       <c r="AT32" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="AU32" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="AV32">
         <v>180</v>
@@ -5100,7 +5119,7 @@
         <v>254</v>
       </c>
       <c r="BA32" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="BD32">
         <v>2734</v>
@@ -5109,54 +5128,54 @@
         <v>2733</v>
       </c>
       <c r="BF32" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="BG32" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B33" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C33" t="s">
         <v>2</v>
       </c>
       <c r="D33" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E33" t="s">
         <v>2</v>
       </c>
       <c r="F33" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G33" t="s">
         <v>2</v>
       </c>
       <c r="H33" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="I33" t="s">
         <v>6</v>
       </c>
       <c r="J33" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="K33" t="s">
         <v>6</v>
       </c>
       <c r="L33" t="s">
-        <v>163</v>
-      </c>
-      <c r="Y33" t="s">
-        <v>187</v>
+        <v>164</v>
+      </c>
+      <c r="Y33" s="1" t="s">
+        <v>170</v>
       </c>
       <c r="Z33" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AA33">
         <v>180</v>
@@ -5174,10 +5193,10 @@
         <v>254</v>
       </c>
       <c r="AF33" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AG33" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="AH33">
         <v>180</v>
@@ -5195,10 +5214,10 @@
         <v>254</v>
       </c>
       <c r="AM33" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AN33" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AO33">
         <v>180</v>
@@ -5216,10 +5235,10 @@
         <v>254</v>
       </c>
       <c r="AT33" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="AU33" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AV33">
         <v>180</v>
@@ -5237,7 +5256,7 @@
         <v>254</v>
       </c>
       <c r="BA33" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="BD33">
         <v>2735</v>
@@ -5246,45 +5265,45 @@
         <v>2733</v>
       </c>
       <c r="BF33" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="BG33" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="34" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B34" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C34" t="s">
         <v>2</v>
       </c>
       <c r="D34" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E34" t="s">
         <v>2</v>
       </c>
       <c r="F34" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G34" t="s">
         <v>2</v>
       </c>
       <c r="H34" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="X34" t="s">
-        <v>72</v>
-      </c>
-      <c r="Y34" t="s">
-        <v>170</v>
+        <v>76</v>
+      </c>
+      <c r="Y34" s="1" t="s">
+        <v>190</v>
       </c>
       <c r="Z34" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AA34">
         <v>170</v>
@@ -5302,10 +5321,10 @@
         <v>254</v>
       </c>
       <c r="AF34" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AG34" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="AH34">
         <v>170</v>
@@ -5323,10 +5342,10 @@
         <v>254</v>
       </c>
       <c r="AM34" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AN34" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="AO34">
         <v>170</v>
@@ -5344,10 +5363,10 @@
         <v>254</v>
       </c>
       <c r="AT34" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="AU34" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="AV34">
         <v>170</v>
@@ -5365,51 +5384,51 @@
         <v>254</v>
       </c>
       <c r="BA34" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="BD34">
         <v>2727</v>
       </c>
       <c r="BF34" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="35" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B35" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C35" t="s">
         <v>2</v>
       </c>
       <c r="D35" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E35" t="s">
         <v>2</v>
       </c>
       <c r="F35" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G35" t="s">
         <v>2</v>
       </c>
       <c r="H35" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="I35" t="s">
         <v>6</v>
       </c>
       <c r="J35" t="s">
-        <v>150</v>
-      </c>
-      <c r="Y35" t="s">
+        <v>151</v>
+      </c>
+      <c r="Y35" s="1" t="s">
         <v>172</v>
       </c>
       <c r="Z35" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AA35">
         <v>150</v>
@@ -5427,10 +5446,10 @@
         <v>254</v>
       </c>
       <c r="AF35" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AG35" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="AH35">
         <v>150</v>
@@ -5448,10 +5467,10 @@
         <v>254</v>
       </c>
       <c r="AM35" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AN35" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="AO35">
         <v>150</v>
@@ -5469,10 +5488,10 @@
         <v>254</v>
       </c>
       <c r="AT35" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="AU35" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="AV35">
         <v>150</v>
@@ -5490,7 +5509,7 @@
         <v>254</v>
       </c>
       <c r="BA35" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="BD35">
         <v>2729</v>
@@ -5499,48 +5518,48 @@
         <v>2727</v>
       </c>
       <c r="BF35" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BG35" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="36" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B36" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C36" t="s">
         <v>2</v>
       </c>
       <c r="D36" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E36" t="s">
         <v>2</v>
       </c>
       <c r="F36" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G36" t="s">
         <v>2</v>
       </c>
       <c r="H36" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="I36" t="s">
         <v>6</v>
       </c>
       <c r="J36" t="s">
-        <v>152</v>
-      </c>
-      <c r="Y36" t="s">
+        <v>153</v>
+      </c>
+      <c r="Y36" s="1" t="s">
         <v>174</v>
       </c>
       <c r="Z36" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AA36">
         <v>170</v>
@@ -5558,10 +5577,10 @@
         <v>254</v>
       </c>
       <c r="AF36" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AG36" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="AH36">
         <v>170</v>
@@ -5579,10 +5598,10 @@
         <v>254</v>
       </c>
       <c r="AM36" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AN36" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="AO36">
         <v>170</v>
@@ -5600,10 +5619,10 @@
         <v>254</v>
       </c>
       <c r="AT36" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="AU36" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="AV36">
         <v>170</v>
@@ -5621,7 +5640,7 @@
         <v>254</v>
       </c>
       <c r="BA36" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="BD36">
         <v>2728</v>
@@ -5630,48 +5649,48 @@
         <v>2727</v>
       </c>
       <c r="BF36" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="BG36" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="37" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="B37" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C37" t="s">
         <v>2</v>
       </c>
       <c r="D37" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E37" t="s">
         <v>2</v>
       </c>
       <c r="F37" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G37" t="s">
         <v>2</v>
       </c>
       <c r="H37" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="I37" t="s">
         <v>6</v>
       </c>
       <c r="J37" t="s">
-        <v>151</v>
-      </c>
-      <c r="Y37" t="s">
-        <v>173</v>
+        <v>152</v>
+      </c>
+      <c r="Y37" s="1" t="s">
+        <v>178</v>
       </c>
       <c r="Z37" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AA37">
         <v>10</v>
@@ -5689,10 +5708,10 @@
         <v>254</v>
       </c>
       <c r="AF37" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AG37" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AH37">
         <v>10</v>
@@ -5710,10 +5729,10 @@
         <v>254</v>
       </c>
       <c r="AM37" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AN37" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AO37">
         <v>10</v>
@@ -5731,10 +5750,10 @@
         <v>254</v>
       </c>
       <c r="AT37" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="AU37" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AV37">
         <v>10</v>
@@ -5752,7 +5771,7 @@
         <v>254</v>
       </c>
       <c r="BA37" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="BD37">
         <v>2731</v>
@@ -5761,48 +5780,48 @@
         <v>2727</v>
       </c>
       <c r="BF37" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="BG37" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="38" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B38" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C38" t="s">
         <v>2</v>
       </c>
       <c r="D38" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E38" t="s">
         <v>2</v>
       </c>
       <c r="F38" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G38" t="s">
         <v>2</v>
       </c>
       <c r="H38" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="I38" t="s">
         <v>6</v>
       </c>
       <c r="J38" t="s">
-        <v>153</v>
-      </c>
-      <c r="Y38" t="s">
-        <v>175</v>
+        <v>154</v>
+      </c>
+      <c r="Y38" s="1" t="s">
+        <v>185</v>
       </c>
       <c r="Z38" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AA38">
         <v>7</v>
@@ -5820,10 +5839,10 @@
         <v>254</v>
       </c>
       <c r="AF38" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AG38" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="AH38">
         <v>7</v>
@@ -5841,10 +5860,10 @@
         <v>254</v>
       </c>
       <c r="AM38" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AN38" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="AO38">
         <v>7</v>
@@ -5862,10 +5881,10 @@
         <v>254</v>
       </c>
       <c r="AT38" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="AU38" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="AV38">
         <v>7</v>
@@ -5883,7 +5902,7 @@
         <v>254</v>
       </c>
       <c r="BA38" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="BD38">
         <v>2730</v>
@@ -5892,16 +5911,16 @@
         <v>2727</v>
       </c>
       <c r="BF38" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="BG38" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:BQ38" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:BG38">
-      <sortCondition ref="A1:A38"/>
+  <autoFilter ref="A1:BO41" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:BO41">
+      <sortCondition ref="A1:A41"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>